<commit_message>
Adding reports results display
</commit_message>
<xml_diff>
--- a/TestData/Reports/Reports Test Case.xlsx
+++ b/TestData/Reports/Reports Test Case.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2715E7AB-699A-4249-9F90-DDAB550C5E3C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9A8D17-1B6B-4848-8A75-959A6B8A8555}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="14">
   <si>
     <t>Type</t>
   </si>
@@ -41,14 +41,44 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>Raid</t>
+  </si>
+  <si>
+    <t>Defense</t>
+  </si>
+  <si>
+    <t>Ally</t>
+  </si>
+  <si>
+    <t>Off</t>
+  </si>
+  <si>
+    <t>Def</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -76,8 +106,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,44 +422,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="1" max="1" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>